<commit_message>
Editing report and analyses. Not complete. Need to transition to checking out the enrollment numbers before coming back to modeling.
</commit_message>
<xml_diff>
--- a/raw_summary_statistics.xlsx
+++ b/raw_summary_statistics.xlsx
@@ -419,31 +419,31 @@
         </is>
       </c>
       <c r="B2">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="C2">
         <v>-2.87</v>
       </c>
       <c r="D2">
-        <v>7.85</v>
+        <v>18.93</v>
       </c>
       <c r="E2">
-        <v>1.19</v>
+        <v>1.35</v>
       </c>
       <c r="F2">
-        <v>0.7</v>
+        <v>0.73</v>
       </c>
       <c r="G2">
-        <v>1.78</v>
+        <v>2.27</v>
       </c>
       <c r="H2">
-        <v>2.23</v>
+        <v>2.34</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
-        <v>2.234706616729089</v>
+        <v>2.340343958812575</v>
       </c>
     </row>
     <row r="3">
@@ -453,7 +453,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -487,7 +487,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -521,7 +521,7 @@
         </is>
       </c>
       <c r="B5">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -555,7 +555,7 @@
         </is>
       </c>
       <c r="B6">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -564,13 +564,13 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0.33</v>
+        <v>0.34</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -589,7 +589,7 @@
         </is>
       </c>
       <c r="B7">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -598,7 +598,7 @@
         <v>1</v>
       </c>
       <c r="E7">
-        <v>0.4</v>
+        <v>0.39</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -623,7 +623,7 @@
         </is>
       </c>
       <c r="B8">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -657,7 +657,7 @@
         </is>
       </c>
       <c r="B9">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -691,7 +691,7 @@
         </is>
       </c>
       <c r="B10">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -725,7 +725,7 @@
         </is>
       </c>
       <c r="B11">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -734,7 +734,7 @@
         <v>1</v>
       </c>
       <c r="E11">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -759,7 +759,7 @@
         </is>
       </c>
       <c r="B12">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -793,7 +793,7 @@
         </is>
       </c>
       <c r="B13">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="C13">
         <v>-13.67</v>
@@ -802,22 +802,22 @@
         <v>14747.43</v>
       </c>
       <c r="E13">
-        <v>804.79</v>
+        <v>818.99</v>
       </c>
       <c r="F13">
-        <v>188.95</v>
+        <v>189.05</v>
       </c>
       <c r="G13">
-        <v>2319.21</v>
+        <v>2312.54</v>
       </c>
       <c r="H13">
-        <v>502.43</v>
+        <v>501.69</v>
       </c>
       <c r="I13">
-        <v>26.262</v>
+        <v>27.64283333333334</v>
       </c>
       <c r="J13">
-        <v>528.6904999999999</v>
+        <v>529.3333333333333</v>
       </c>
     </row>
     <row r="14">
@@ -827,7 +827,7 @@
         </is>
       </c>
       <c r="B14">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -836,13 +836,13 @@
         <v>98.7</v>
       </c>
       <c r="E14">
-        <v>1.58</v>
+        <v>1.55</v>
       </c>
       <c r="F14">
         <v>0.2</v>
       </c>
       <c r="G14">
-        <v>9.210000000000001</v>
+        <v>9.1</v>
       </c>
       <c r="H14">
         <v>0.6</v>
@@ -861,7 +861,7 @@
         </is>
       </c>
       <c r="B15">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -870,13 +870,13 @@
         <v>56</v>
       </c>
       <c r="E15">
-        <v>4.08</v>
+        <v>4.16</v>
       </c>
       <c r="F15">
-        <v>1.15</v>
+        <v>1.1</v>
       </c>
       <c r="G15">
-        <v>7.79</v>
+        <v>7.88</v>
       </c>
       <c r="H15">
         <v>3.5</v>
@@ -895,31 +895,31 @@
         </is>
       </c>
       <c r="B16">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16">
-        <v>97.90000000000001</v>
+        <v>99.5</v>
       </c>
       <c r="E16">
-        <v>13.19</v>
+        <v>13.43</v>
       </c>
       <c r="F16">
         <v>3.6</v>
       </c>
       <c r="G16">
-        <v>21.61</v>
+        <v>21.96</v>
       </c>
       <c r="H16">
-        <v>14.55</v>
+        <v>14.78</v>
       </c>
       <c r="I16">
         <v>0.7000000000000001</v>
       </c>
       <c r="J16">
-        <v>15.25</v>
+        <v>15.475</v>
       </c>
     </row>
     <row r="17">
@@ -929,7 +929,7 @@
         </is>
       </c>
       <c r="B17">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -938,22 +938,22 @@
         <v>100</v>
       </c>
       <c r="E17">
-        <v>24.71</v>
+        <v>24.93</v>
       </c>
       <c r="F17">
-        <v>14.4</v>
+        <v>14.45</v>
       </c>
       <c r="G17">
-        <v>25.92</v>
+        <v>26.26</v>
       </c>
       <c r="H17">
-        <v>27.4</v>
+        <v>28.08</v>
       </c>
       <c r="I17">
         <v>6.049999999999999</v>
       </c>
       <c r="J17">
-        <v>33.45</v>
+        <v>34.125</v>
       </c>
     </row>
     <row r="18">
@@ -963,7 +963,7 @@
         </is>
       </c>
       <c r="B18">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -972,13 +972,13 @@
         <v>9.699999999999999</v>
       </c>
       <c r="E18">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
       <c r="F18">
         <v>0</v>
       </c>
       <c r="G18">
-        <v>0.72</v>
+        <v>0.71</v>
       </c>
       <c r="H18">
         <v>0.2</v>
@@ -997,7 +997,7 @@
         </is>
       </c>
       <c r="B19">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1031,7 +1031,7 @@
         </is>
       </c>
       <c r="B20">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -1040,19 +1040,19 @@
         <v>23.8</v>
       </c>
       <c r="E20">
-        <v>3.88</v>
+        <v>3.85</v>
       </c>
       <c r="F20">
-        <v>3.4</v>
+        <v>3.35</v>
       </c>
       <c r="G20">
         <v>3.1</v>
       </c>
       <c r="H20">
-        <v>4</v>
+        <v>4.1</v>
       </c>
       <c r="I20">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="J20">
         <v>5.5</v>
@@ -1065,7 +1065,7 @@
         </is>
       </c>
       <c r="B21">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -1074,22 +1074,22 @@
         <v>97.7</v>
       </c>
       <c r="E21">
-        <v>52.31</v>
+        <v>51.83</v>
       </c>
       <c r="F21">
-        <v>57.25</v>
+        <v>56.95</v>
       </c>
       <c r="G21">
-        <v>31.35</v>
+        <v>31.54</v>
       </c>
       <c r="H21">
-        <v>53.17</v>
+        <v>54.12</v>
       </c>
       <c r="I21">
-        <v>26.875</v>
+        <v>25.875</v>
       </c>
       <c r="J21">
-        <v>80.05</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22">
@@ -1099,7 +1099,7 @@
         </is>
       </c>
       <c r="B22">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c r="C22">
         <v>0.4</v>
@@ -1108,22 +1108,22 @@
         <v>100</v>
       </c>
       <c r="E22">
-        <v>50.45</v>
+        <v>50.83</v>
       </c>
       <c r="F22">
-        <v>49</v>
+        <v>49.2</v>
       </c>
       <c r="G22">
-        <v>28.26</v>
+        <v>28.48</v>
       </c>
       <c r="H22">
-        <v>46.5</v>
+        <v>46.9</v>
       </c>
       <c r="I22">
-        <v>27.5</v>
+        <v>27.7</v>
       </c>
       <c r="J22">
-        <v>74</v>
+        <v>74.59999999999999</v>
       </c>
     </row>
     <row r="23">
@@ -1133,7 +1133,7 @@
         </is>
       </c>
       <c r="B23">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -1142,22 +1142,22 @@
         <v>99.94</v>
       </c>
       <c r="E23">
-        <v>51.55</v>
+        <v>51.64</v>
       </c>
       <c r="F23">
         <v>53.47</v>
       </c>
       <c r="G23">
-        <v>27.89</v>
+        <v>27.98</v>
       </c>
       <c r="H23">
-        <v>48.52</v>
+        <v>48.79</v>
       </c>
       <c r="I23">
         <v>26.86</v>
       </c>
       <c r="J23">
-        <v>75.38</v>
+        <v>75.65000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1247,34 +1247,34 @@
         </is>
       </c>
       <c r="B2">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="C2">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D2">
-        <v>0.425</v>
+        <v>0.607</v>
       </c>
       <c r="E2">
-        <v>1.244</v>
+        <v>1.421</v>
       </c>
       <c r="F2">
-        <v>0.819</v>
+        <v>0.8129999999999999</v>
       </c>
       <c r="G2">
-        <v>1.657</v>
+        <v>2.288</v>
       </c>
       <c r="H2">
-        <v>0.103</v>
+        <v>0.025</v>
       </c>
       <c r="I2">
-        <v>53.321</v>
+        <v>69.10299999999999</v>
       </c>
       <c r="J2">
-        <v>-0.089</v>
+        <v>0.078</v>
       </c>
       <c r="K2">
-        <v>0.9399999999999999</v>
+        <v>1.137</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
@@ -1294,34 +1294,34 @@
         </is>
       </c>
       <c r="B3">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="C3">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D3">
-        <v>0.18</v>
+        <v>0.243</v>
       </c>
       <c r="E3">
-        <v>1.24</v>
+        <v>1.412</v>
       </c>
       <c r="F3">
-        <v>1.06</v>
+        <v>1.17</v>
       </c>
       <c r="G3">
-        <v>0.8179999999999999</v>
+        <v>0.962</v>
       </c>
       <c r="H3">
-        <v>0.415</v>
+        <v>0.337</v>
       </c>
       <c r="I3">
-        <v>150.689</v>
+        <v>191.109</v>
       </c>
       <c r="J3">
         <v>-0.255</v>
       </c>
       <c r="K3">
-        <v>0.615</v>
+        <v>0.74</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
@@ -1341,34 +1341,34 @@
         </is>
       </c>
       <c r="B4">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="C4">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D4">
-        <v>0.223</v>
+        <v>0.392</v>
       </c>
       <c r="E4">
-        <v>1.253</v>
+        <v>1.452</v>
       </c>
       <c r="F4">
-        <v>1.029</v>
+        <v>1.061</v>
       </c>
       <c r="G4">
-        <v>1.074</v>
+        <v>1.687</v>
       </c>
       <c r="H4">
-        <v>0.285</v>
+        <v>0.093</v>
       </c>
       <c r="I4">
-        <v>173.795</v>
+        <v>235.698</v>
       </c>
       <c r="J4">
-        <v>-0.187</v>
+        <v>-0.066</v>
       </c>
       <c r="K4">
-        <v>0.634</v>
+        <v>0.849</v>
       </c>
       <c r="L4" t="inlineStr">
         <is>
@@ -1388,34 +1388,34 @@
         </is>
       </c>
       <c r="B5">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="C5">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D5">
-        <v>0.458</v>
+        <v>0.57</v>
       </c>
       <c r="E5">
-        <v>1.251</v>
+        <v>1.423</v>
       </c>
       <c r="F5">
-        <v>0.793</v>
+        <v>0.854</v>
       </c>
       <c r="G5">
-        <v>1.415</v>
+        <v>1.751</v>
       </c>
       <c r="H5">
-        <v>0.163</v>
+        <v>0.08500000000000001</v>
       </c>
       <c r="I5">
-        <v>47.55</v>
+        <v>60.423</v>
       </c>
       <c r="J5">
-        <v>-0.193</v>
+        <v>-0.081</v>
       </c>
       <c r="K5">
-        <v>1.108</v>
+        <v>1.22</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
@@ -1435,34 +1435,34 @@
         </is>
       </c>
       <c r="B6">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="C6">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D6">
-        <v>0.133</v>
+        <v>0.264</v>
       </c>
       <c r="E6">
-        <v>1.247</v>
+        <v>1.453</v>
       </c>
       <c r="F6">
-        <v>1.114</v>
+        <v>1.189</v>
       </c>
       <c r="G6">
-        <v>0.663</v>
+        <v>1.104</v>
       </c>
       <c r="H6">
-        <v>0.508</v>
+        <v>0.27</v>
       </c>
       <c r="I6">
-        <v>286.56</v>
+        <v>319.582</v>
       </c>
       <c r="J6">
-        <v>-0.261</v>
+        <v>-0.207</v>
       </c>
       <c r="K6">
-        <v>0.527</v>
+        <v>0.735</v>
       </c>
       <c r="L6" t="inlineStr">
         <is>
@@ -1482,34 +1482,34 @@
         </is>
       </c>
       <c r="B7">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="C7">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D7">
-        <v>0.178</v>
+        <v>0.317</v>
       </c>
       <c r="E7">
-        <v>1.245</v>
+        <v>1.44</v>
       </c>
       <c r="F7">
-        <v>1.067</v>
+        <v>1.124</v>
       </c>
       <c r="G7">
-        <v>0.86</v>
+        <v>1.325</v>
       </c>
       <c r="H7">
-        <v>0.391</v>
+        <v>0.187</v>
       </c>
       <c r="I7">
-        <v>192.197</v>
+        <v>243.955</v>
       </c>
       <c r="J7">
-        <v>-0.23</v>
+        <v>-0.154</v>
       </c>
       <c r="K7">
-        <v>0.586</v>
+        <v>0.787</v>
       </c>
       <c r="L7" t="inlineStr">
         <is>
@@ -1529,34 +1529,34 @@
         </is>
       </c>
       <c r="B8">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="C8">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D8">
-        <v>0.198</v>
+        <v>0.301</v>
       </c>
       <c r="E8">
-        <v>1.257</v>
+        <v>1.445</v>
       </c>
       <c r="F8">
-        <v>1.059</v>
+        <v>1.144</v>
       </c>
       <c r="G8">
-        <v>0.973</v>
+        <v>1.263</v>
       </c>
       <c r="H8">
-        <v>0.331</v>
+        <v>0.207</v>
       </c>
       <c r="I8">
-        <v>223.945</v>
+        <v>275.203</v>
       </c>
       <c r="J8">
-        <v>-0.203</v>
+        <v>-0.168</v>
       </c>
       <c r="K8">
-        <v>0.598</v>
+        <v>0.769</v>
       </c>
       <c r="L8" t="inlineStr">
         <is>
@@ -1576,34 +1576,34 @@
         </is>
       </c>
       <c r="B9">
-        <v>238</v>
+        <v>244</v>
       </c>
       <c r="C9">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D9">
-        <v>-0.228</v>
+        <v>-0.049</v>
       </c>
       <c r="E9">
-        <v>1.138</v>
+        <v>1.337</v>
       </c>
       <c r="F9">
-        <v>1.366</v>
+        <v>1.386</v>
       </c>
       <c r="G9">
-        <v>-1.063</v>
+        <v>-0.206</v>
       </c>
       <c r="H9">
-        <v>0.289</v>
+        <v>0.837</v>
       </c>
       <c r="I9">
-        <v>150.564</v>
+        <v>207.32</v>
       </c>
       <c r="J9">
-        <v>-0.651</v>
+        <v>-0.515</v>
       </c>
       <c r="K9">
-        <v>0.195</v>
+        <v>0.418</v>
       </c>
       <c r="L9" t="inlineStr">
         <is>
@@ -1623,34 +1623,34 @@
         </is>
       </c>
       <c r="B10">
-        <v>301</v>
+        <v>308</v>
       </c>
       <c r="C10">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D10">
-        <v>0.374</v>
+        <v>0.581</v>
       </c>
       <c r="E10">
-        <v>1.211</v>
+        <v>1.376</v>
       </c>
       <c r="F10">
-        <v>0.837</v>
+        <v>0.796</v>
       </c>
       <c r="G10">
-        <v>0.804</v>
+        <v>1.308</v>
       </c>
       <c r="H10">
-        <v>0.435</v>
+        <v>0.208</v>
       </c>
       <c r="I10">
-        <v>14.369</v>
+        <v>16.767</v>
       </c>
       <c r="J10">
-        <v>-0.621</v>
+        <v>-0.357</v>
       </c>
       <c r="K10">
-        <v>1.369</v>
+        <v>1.518</v>
       </c>
       <c r="L10" t="inlineStr">
         <is>
@@ -1670,34 +1670,34 @@
         </is>
       </c>
       <c r="B11">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="C11">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D11">
-        <v>0.295</v>
+        <v>0.529</v>
       </c>
       <c r="E11">
-        <v>1.287</v>
+        <v>1.513</v>
       </c>
       <c r="F11">
-        <v>0.992</v>
+        <v>0.984</v>
       </c>
       <c r="G11">
-        <v>1.486</v>
+        <v>2.344</v>
       </c>
       <c r="H11">
-        <v>0.139</v>
+        <v>0.02</v>
       </c>
       <c r="I11">
-        <v>234.422</v>
+        <v>296.367</v>
       </c>
       <c r="J11">
-        <v>-0.096</v>
+        <v>0.08500000000000001</v>
       </c>
       <c r="K11">
-        <v>0.6860000000000001</v>
+        <v>0.974</v>
       </c>
       <c r="L11" t="inlineStr">
         <is>
@@ -1765,16 +1765,16 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>118.4011847082842</v>
+        <v>154.4598779729278</v>
       </c>
       <c r="D2">
-        <v>39.46706156942805</v>
+        <v>51.48662599097594</v>
       </c>
       <c r="E2">
-        <v>14.01321851643154</v>
+        <v>10.9615182896583</v>
       </c>
       <c r="F2">
-        <v>1.364254211974835e-08</v>
+        <v>7.186355722274816e-07</v>
       </c>
     </row>
     <row r="3">
@@ -1787,16 +1787,16 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>4.204201248483636</v>
+        <v>9.759004555692567</v>
       </c>
       <c r="D3">
-        <v>1.051050312120909</v>
+        <v>2.439751138923142</v>
       </c>
       <c r="E3">
-        <v>0.3290826750367163</v>
+        <v>0.4721941557990477</v>
       </c>
       <c r="F3">
-        <v>0.8583529801424807</v>
+        <v>0.7561471833188502</v>
       </c>
     </row>
     <row r="4">
@@ -1809,16 +1809,16 @@
         <v>19</v>
       </c>
       <c r="C4">
-        <v>310.2901090562785</v>
+        <v>413.7763613511093</v>
       </c>
       <c r="D4">
-        <v>16.33105837138308</v>
+        <v>21.77770322900575</v>
       </c>
       <c r="E4">
-        <v>7.043194419655037</v>
+        <v>5.325621312230179</v>
       </c>
       <c r="F4">
-        <v>1.867827595169419e-15</v>
+        <v>3.772747684233216e-11</v>
       </c>
     </row>
   </sheetData>
@@ -1888,22 +1888,22 @@
         </is>
       </c>
       <c r="B2">
-        <v>0.007</v>
+        <v>0.018</v>
       </c>
       <c r="C2">
-        <v>0.116</v>
+        <v>0.325</v>
       </c>
       <c r="D2">
-        <v>0.908</v>
+        <v>0.745</v>
       </c>
       <c r="E2">
-        <v>313</v>
+        <v>321</v>
       </c>
       <c r="F2">
-        <v>-0.104</v>
+        <v>-0.091</v>
       </c>
       <c r="G2">
-        <v>0.117</v>
+        <v>0.127</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -1926,19 +1926,19 @@
         <v>-0.047</v>
       </c>
       <c r="C3">
-        <v>-0.832</v>
+        <v>-0.845</v>
       </c>
       <c r="D3">
-        <v>0.406</v>
+        <v>0.398</v>
       </c>
       <c r="E3">
-        <v>310</v>
+        <v>318</v>
       </c>
       <c r="F3">
-        <v>-0.157</v>
+        <v>-0.156</v>
       </c>
       <c r="G3">
-        <v>0.064</v>
+        <v>0.063</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -1958,22 +1958,22 @@
         </is>
       </c>
       <c r="B4">
-        <v>0.013</v>
+        <v>0.006</v>
       </c>
       <c r="C4">
-        <v>0.224</v>
+        <v>0.113</v>
       </c>
       <c r="D4">
-        <v>0.823</v>
+        <v>0.91</v>
       </c>
       <c r="E4">
-        <v>310</v>
+        <v>318</v>
       </c>
       <c r="F4">
-        <v>-0.098</v>
+        <v>-0.103</v>
       </c>
       <c r="G4">
-        <v>0.124</v>
+        <v>0.116</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -1993,22 +1993,22 @@
         </is>
       </c>
       <c r="B5">
-        <v>-0.005</v>
+        <v>-0.013</v>
       </c>
       <c r="C5">
-        <v>-0.083</v>
+        <v>-0.224</v>
       </c>
       <c r="D5">
-        <v>0.9340000000000001</v>
+        <v>0.823</v>
       </c>
       <c r="E5">
-        <v>310</v>
+        <v>318</v>
       </c>
       <c r="F5">
-        <v>-0.116</v>
+        <v>-0.122</v>
       </c>
       <c r="G5">
-        <v>0.106</v>
+        <v>0.097</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -2028,22 +2028,22 @@
         </is>
       </c>
       <c r="B6">
-        <v>0.06900000000000001</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="C6">
-        <v>1.209</v>
+        <v>1.569</v>
       </c>
       <c r="D6">
-        <v>0.228</v>
+        <v>0.118</v>
       </c>
       <c r="E6">
-        <v>310</v>
+        <v>318</v>
       </c>
       <c r="F6">
-        <v>-0.043</v>
+        <v>-0.022</v>
       </c>
       <c r="G6">
-        <v>0.178</v>
+        <v>0.195</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -2063,22 +2063,22 @@
         </is>
       </c>
       <c r="B7">
-        <v>-0.092</v>
+        <v>-0.093</v>
       </c>
       <c r="C7">
-        <v>-1.633</v>
+        <v>-1.668</v>
       </c>
       <c r="D7">
-        <v>0.103</v>
+        <v>0.096</v>
       </c>
       <c r="E7">
-        <v>310</v>
+        <v>318</v>
       </c>
       <c r="F7">
         <v>-0.201</v>
       </c>
       <c r="G7">
-        <v>0.019</v>
+        <v>0.017</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -2098,22 +2098,22 @@
         </is>
       </c>
       <c r="B8">
-        <v>-0.09</v>
+        <v>-0.078</v>
       </c>
       <c r="C8">
-        <v>-1.588</v>
+        <v>-1.387</v>
       </c>
       <c r="D8">
-        <v>0.113</v>
+        <v>0.167</v>
       </c>
       <c r="E8">
-        <v>310</v>
+        <v>318</v>
       </c>
       <c r="F8">
-        <v>-0.199</v>
+        <v>-0.186</v>
       </c>
       <c r="G8">
-        <v>0.021</v>
+        <v>0.032</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -2133,22 +2133,22 @@
         </is>
       </c>
       <c r="B9">
-        <v>-0.012</v>
+        <v>-0.039</v>
       </c>
       <c r="C9">
-        <v>-0.21</v>
+        <v>-0.7</v>
       </c>
       <c r="D9">
-        <v>0.834</v>
+        <v>0.484</v>
       </c>
       <c r="E9">
-        <v>310</v>
+        <v>318</v>
       </c>
       <c r="F9">
-        <v>-0.123</v>
+        <v>-0.148</v>
       </c>
       <c r="G9">
-        <v>0.099</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
@@ -2168,22 +2168,22 @@
         </is>
       </c>
       <c r="B10">
-        <v>-0.039</v>
+        <v>-0.046</v>
       </c>
       <c r="C10">
-        <v>-0.6889999999999999</v>
+        <v>-0.821</v>
       </c>
       <c r="D10">
-        <v>0.491</v>
+        <v>0.412</v>
       </c>
       <c r="E10">
-        <v>310</v>
+        <v>318</v>
       </c>
       <c r="F10">
-        <v>-0.15</v>
+        <v>-0.155</v>
       </c>
       <c r="G10">
-        <v>0.07199999999999999</v>
+        <v>0.064</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
@@ -2203,22 +2203,22 @@
         </is>
       </c>
       <c r="B11">
-        <v>0.023</v>
+        <v>0.016</v>
       </c>
       <c r="C11">
-        <v>0.392</v>
+        <v>0.276</v>
       </c>
       <c r="D11">
-        <v>0.695</v>
+        <v>0.782</v>
       </c>
       <c r="E11">
-        <v>303</v>
+        <v>311</v>
       </c>
       <c r="F11">
-        <v>-0.09</v>
+        <v>-0.095</v>
       </c>
       <c r="G11">
-        <v>0.135</v>
+        <v>0.126</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
@@ -2238,22 +2238,22 @@
         </is>
       </c>
       <c r="B12">
-        <v>0.062</v>
+        <v>0.052</v>
       </c>
       <c r="C12">
-        <v>1.096</v>
+        <v>0.93</v>
       </c>
       <c r="D12">
-        <v>0.274</v>
+        <v>0.353</v>
       </c>
       <c r="E12">
-        <v>313</v>
+        <v>321</v>
       </c>
       <c r="F12">
-        <v>-0.049</v>
+        <v>-0.058</v>
       </c>
       <c r="G12">
-        <v>0.171</v>
+        <v>0.16</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>

</xml_diff>